<commit_message>
added new results for specific fault locations; edited get_pf_shortcircuit_results.py
</commit_message>
<xml_diff>
--- a/pandapower/test/shortcircuit/SCE_Tests/sc_result_comparison/test_case_1_four_bus_radial_grid_pf_sc_results_bus.xlsx
+++ b/pandapower/test/shortcircuit/SCE_Tests/sc_result_comparison/test_case_1_four_bus_radial_grid_pf_sc_results_bus.xlsx
@@ -23,22 +23,22 @@
     <sheet name="LL_min_10" sheetId="14" r:id="rId14"/>
     <sheet name="LL_min_fault_6" sheetId="15" r:id="rId15"/>
     <sheet name="LL_min_fault_10" sheetId="16" r:id="rId16"/>
-    <sheet name="LLG_max_6" sheetId="17" r:id="rId17"/>
-    <sheet name="LLG_max_10" sheetId="18" r:id="rId18"/>
-    <sheet name="LLG_max_fault_6" sheetId="19" r:id="rId19"/>
-    <sheet name="LLG_max_fault_10" sheetId="20" r:id="rId20"/>
-    <sheet name="LLG_min_6" sheetId="21" r:id="rId21"/>
-    <sheet name="LLG_min_10" sheetId="22" r:id="rId22"/>
-    <sheet name="LLG_min_fault_6" sheetId="23" r:id="rId23"/>
-    <sheet name="LLG_min_fault_10" sheetId="24" r:id="rId24"/>
-    <sheet name="LG_max_6" sheetId="25" r:id="rId25"/>
-    <sheet name="LG_max_10" sheetId="26" r:id="rId26"/>
-    <sheet name="LG_max_fault_6" sheetId="27" r:id="rId27"/>
-    <sheet name="LG_max_fault_10" sheetId="28" r:id="rId28"/>
-    <sheet name="LG_min_6" sheetId="29" r:id="rId29"/>
-    <sheet name="LG_min_10" sheetId="30" r:id="rId30"/>
-    <sheet name="LG_min_fault_6" sheetId="31" r:id="rId31"/>
-    <sheet name="LG_min_fault_10" sheetId="32" r:id="rId32"/>
+    <sheet name="LG_max_6" sheetId="17" r:id="rId17"/>
+    <sheet name="LG_max_10" sheetId="18" r:id="rId18"/>
+    <sheet name="LG_max_fault_6" sheetId="19" r:id="rId19"/>
+    <sheet name="LG_max_fault_10" sheetId="20" r:id="rId20"/>
+    <sheet name="LG_min_6" sheetId="21" r:id="rId21"/>
+    <sheet name="LG_min_10" sheetId="22" r:id="rId22"/>
+    <sheet name="LG_min_fault_6" sheetId="23" r:id="rId23"/>
+    <sheet name="LG_min_fault_10" sheetId="24" r:id="rId24"/>
+    <sheet name="LLG_max_6" sheetId="25" r:id="rId25"/>
+    <sheet name="LLG_max_10" sheetId="26" r:id="rId26"/>
+    <sheet name="LLG_max_fault_6" sheetId="27" r:id="rId27"/>
+    <sheet name="LLG_max_fault_10" sheetId="28" r:id="rId28"/>
+    <sheet name="LLG_min_6" sheetId="29" r:id="rId29"/>
+    <sheet name="LLG_min_10" sheetId="30" r:id="rId30"/>
+    <sheet name="LLG_min_fault_6" sheetId="31" r:id="rId31"/>
+    <sheet name="LLG_min_fault_10" sheetId="32" r:id="rId32"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -2843,58 +2843,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2.881307834727568</v>
       </c>
       <c r="C2">
-        <v>2.884527493204643</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>2.883549636712145</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>33.27047707996278</v>
       </c>
       <c r="F2">
-        <v>33.30765449373155</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>33.29636317954809</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.4428835862221404</v>
+        <v>0.4428835862221607</v>
       </c>
       <c r="I2">
-        <v>4.40271973851942</v>
+        <v>4.402719738519057</v>
       </c>
       <c r="J2">
-        <v>0.4378163569293868</v>
+        <v>0.437816356924225</v>
       </c>
       <c r="K2">
-        <v>4.378163482534344</v>
+        <v>4.378163482487345</v>
       </c>
       <c r="L2">
-        <v>0.4378163569022844</v>
+        <v>0.4378163569023265</v>
       </c>
       <c r="M2">
-        <v>4.378163482487168</v>
+        <v>4.378163482487091</v>
       </c>
       <c r="N2">
-        <v>0.636280712791619</v>
+        <v>0.6355772023502927</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1.1000000238379</v>
       </c>
       <c r="P2">
-        <v>0.6362807127881797</v>
+        <v>0.6357927364583869</v>
       </c>
       <c r="Q2">
-        <v>-0.01117384664767678</v>
+        <v>59.90088731360098</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>-89.99999999999633</v>
       </c>
       <c r="S2">
-        <v>179.9888261535143</v>
+        <v>120.0878544346237</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -2902,58 +2902,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2.248943182936928</v>
       </c>
       <c r="C3">
-        <v>2.659777356923221</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>2.088302030918968</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>25.96855904121619</v>
       </c>
       <c r="F3">
-        <v>30.71246346008186</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>24.11363479400617</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>4.185910274912399</v>
+        <v>4.185910274912456</v>
       </c>
       <c r="I3">
-        <v>5.870495034006284</v>
+        <v>5.870495034005926</v>
       </c>
       <c r="J3">
-        <v>0.9578163680532483</v>
+        <v>0.9578163680481669</v>
       </c>
       <c r="K3">
-        <v>4.968163485641733</v>
+        <v>4.968163485594707</v>
       </c>
       <c r="L3">
-        <v>0.9578163680261339</v>
+        <v>0.9578163680263008</v>
       </c>
       <c r="M3">
-        <v>4.968163485594578</v>
+        <v>4.968163485594511</v>
       </c>
       <c r="N3">
-        <v>0.7178088853018512</v>
+        <v>0.5967063269904345</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>1.100000023838578</v>
       </c>
       <c r="P3">
-        <v>0.7178088852998012</v>
+        <v>0.7599982922815229</v>
       </c>
       <c r="Q3">
-        <v>-6.313450644998808</v>
+        <v>48.84809195671546</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>-89.99999999999643</v>
       </c>
       <c r="S3">
-        <v>173.6865493550667</v>
+        <v>121.109045449341</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -2961,58 +2961,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1.780157175146007</v>
       </c>
       <c r="C4">
-        <v>2.314120905097126</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1.728412445116583</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>20.55548448540782</v>
       </c>
       <c r="F4">
-        <v>26.72116654990332</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>19.95798780917517</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>7.895175922947225</v>
+        <v>7.895175922947306</v>
       </c>
       <c r="I4">
-        <v>7.335082718453467</v>
+        <v>7.335082718453107</v>
       </c>
       <c r="J4">
-        <v>1.477816378918005</v>
+        <v>1.477816378913027</v>
       </c>
       <c r="K4">
-        <v>5.558163489027947</v>
+        <v>5.558163488980915</v>
       </c>
       <c r="L4">
-        <v>1.477816378890885</v>
+        <v>1.477816378891169</v>
       </c>
       <c r="M4">
-        <v>5.558163488980837</v>
+        <v>5.558163488980771</v>
       </c>
       <c r="N4">
-        <v>0.7719945678108373</v>
+        <v>0.6175627786591105</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1.100000023839263</v>
       </c>
       <c r="P4">
-        <v>0.7719945678096874</v>
+        <v>0.826836754355374</v>
       </c>
       <c r="Q4">
-        <v>-6.619958059522241</v>
+        <v>41.92164926482276</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>-89.9999999999964</v>
       </c>
       <c r="S4">
-        <v>173.3800419405132</v>
+        <v>123.7614475143174</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -3020,58 +3020,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1.780157175146008</v>
       </c>
       <c r="C5">
-        <v>2.314120905097127</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>1.728412445116581</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>20.55548448540783</v>
       </c>
       <c r="F5">
-        <v>26.72116654990333</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>19.95798780917515</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>7.895175922947224</v>
+        <v>7.895175922947299</v>
       </c>
       <c r="I5">
-        <v>7.335082718453457</v>
+        <v>7.335082718453101</v>
       </c>
       <c r="J5">
-        <v>1.477816378918004</v>
+        <v>1.477816378913028</v>
       </c>
       <c r="K5">
-        <v>5.558163489027946</v>
+        <v>5.558163488980913</v>
       </c>
       <c r="L5">
-        <v>1.477816378890884</v>
+        <v>1.477816378891169</v>
       </c>
       <c r="M5">
-        <v>5.558163488980837</v>
+        <v>5.558163488980769</v>
       </c>
       <c r="N5">
-        <v>0.7719945678108373</v>
+        <v>0.6175627786591099</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1.100000023839263</v>
       </c>
       <c r="P5">
-        <v>0.7719945678096877</v>
+        <v>0.8268367543553737</v>
       </c>
       <c r="Q5">
-        <v>-6.619958059522241</v>
+        <v>41.92164926482278</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>-89.99999999999639</v>
       </c>
       <c r="S5">
-        <v>173.3800419405131</v>
+        <v>123.7614475143174</v>
       </c>
     </row>
   </sheetData>
@@ -3151,58 +3151,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2.881307834727568</v>
       </c>
       <c r="C2">
-        <v>2.884527493204643</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>2.883549636712145</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>33.27047707996278</v>
       </c>
       <c r="F2">
-        <v>33.30765449373155</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>33.29636317954809</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.4428835862221404</v>
+        <v>0.4428835862221607</v>
       </c>
       <c r="I2">
-        <v>4.40271973851942</v>
+        <v>4.402719738519057</v>
       </c>
       <c r="J2">
-        <v>0.4378163569293868</v>
+        <v>0.437816356924225</v>
       </c>
       <c r="K2">
-        <v>4.378163482534344</v>
+        <v>4.378163482487345</v>
       </c>
       <c r="L2">
-        <v>0.4378163569022844</v>
+        <v>0.4378163569023265</v>
       </c>
       <c r="M2">
-        <v>4.378163482487168</v>
+        <v>4.378163482487091</v>
       </c>
       <c r="N2">
-        <v>0.636280712791619</v>
+        <v>0.6355772023502927</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1.1000000238379</v>
       </c>
       <c r="P2">
-        <v>0.6362807127881797</v>
+        <v>0.6357927364583869</v>
       </c>
       <c r="Q2">
-        <v>-0.01117384664767678</v>
+        <v>59.90088731360098</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>-89.99999999999633</v>
       </c>
       <c r="S2">
-        <v>179.9888261535143</v>
+        <v>120.0878544346237</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -3210,58 +3210,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2.248943182936928</v>
       </c>
       <c r="C3">
-        <v>2.659777356923221</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>2.088302030918968</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>25.96855904121619</v>
       </c>
       <c r="F3">
-        <v>30.71246346008186</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>24.11363479400617</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>4.185910274912399</v>
+        <v>4.185910274912456</v>
       </c>
       <c r="I3">
-        <v>5.870495034006284</v>
+        <v>5.870495034005926</v>
       </c>
       <c r="J3">
-        <v>0.9578163680532483</v>
+        <v>0.9578163680481669</v>
       </c>
       <c r="K3">
-        <v>4.968163485641733</v>
+        <v>4.968163485594707</v>
       </c>
       <c r="L3">
-        <v>0.9578163680261339</v>
+        <v>0.9578163680263008</v>
       </c>
       <c r="M3">
-        <v>4.968163485594578</v>
+        <v>4.968163485594511</v>
       </c>
       <c r="N3">
-        <v>0.7178088853018512</v>
+        <v>0.5967063269904345</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>1.100000023838578</v>
       </c>
       <c r="P3">
-        <v>0.7178088852998012</v>
+        <v>0.7599982922815229</v>
       </c>
       <c r="Q3">
-        <v>-6.313450644998808</v>
+        <v>48.84809195671546</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>-89.99999999999643</v>
       </c>
       <c r="S3">
-        <v>173.6865493550667</v>
+        <v>121.109045449341</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -3269,58 +3269,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1.780157175146007</v>
       </c>
       <c r="C4">
-        <v>2.314120905097126</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1.728412445116583</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>20.55548448540782</v>
       </c>
       <c r="F4">
-        <v>26.72116654990332</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>19.95798780917517</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>7.895175922947225</v>
+        <v>7.895175922947306</v>
       </c>
       <c r="I4">
-        <v>7.335082718453467</v>
+        <v>7.335082718453107</v>
       </c>
       <c r="J4">
-        <v>1.477816378918005</v>
+        <v>1.477816378913027</v>
       </c>
       <c r="K4">
-        <v>5.558163489027947</v>
+        <v>5.558163488980915</v>
       </c>
       <c r="L4">
-        <v>1.477816378890885</v>
+        <v>1.477816378891169</v>
       </c>
       <c r="M4">
-        <v>5.558163488980837</v>
+        <v>5.558163488980771</v>
       </c>
       <c r="N4">
-        <v>0.7719945678108373</v>
+        <v>0.6175627786591105</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1.100000023839263</v>
       </c>
       <c r="P4">
-        <v>0.7719945678096874</v>
+        <v>0.826836754355374</v>
       </c>
       <c r="Q4">
-        <v>-6.619958059522241</v>
+        <v>41.92164926482276</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>-89.9999999999964</v>
       </c>
       <c r="S4">
-        <v>173.3800419405132</v>
+        <v>123.7614475143174</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -3328,58 +3328,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1.780157175146008</v>
       </c>
       <c r="C5">
-        <v>2.314120905097127</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>1.728412445116581</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>20.55548448540783</v>
       </c>
       <c r="F5">
-        <v>26.72116654990333</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>19.95798780917515</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>7.895175922947224</v>
+        <v>7.895175922947299</v>
       </c>
       <c r="I5">
-        <v>7.335082718453457</v>
+        <v>7.335082718453101</v>
       </c>
       <c r="J5">
-        <v>1.477816378918004</v>
+        <v>1.477816378913028</v>
       </c>
       <c r="K5">
-        <v>5.558163489027946</v>
+        <v>5.558163488980913</v>
       </c>
       <c r="L5">
-        <v>1.477816378890884</v>
+        <v>1.477816378891169</v>
       </c>
       <c r="M5">
-        <v>5.558163488980837</v>
+        <v>5.558163488980769</v>
       </c>
       <c r="N5">
-        <v>0.7719945678108373</v>
+        <v>0.6175627786591099</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1.100000023839263</v>
       </c>
       <c r="P5">
-        <v>0.7719945678096877</v>
+        <v>0.8268367543553737</v>
       </c>
       <c r="Q5">
-        <v>-6.619958059522241</v>
+        <v>41.92164926482278</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>-89.99999999999639</v>
       </c>
       <c r="S5">
-        <v>173.3800419405131</v>
+        <v>123.7614475143174</v>
       </c>
     </row>
   </sheetData>
@@ -3459,58 +3459,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1.170817013876365</v>
       </c>
       <c r="C2">
-        <v>1.170998762980853</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1.171492593911478</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>13.51943036266627</v>
       </c>
       <c r="F2">
-        <v>13.52152902055428</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>13.5272312889689</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.4428835862221404</v>
+        <v>0.4428835862221607</v>
       </c>
       <c r="I2">
-        <v>4.40271973851942</v>
+        <v>4.402719738519057</v>
       </c>
       <c r="J2">
-        <v>0.4378163569293868</v>
+        <v>0.437816356924225</v>
       </c>
       <c r="K2">
-        <v>4.378163482534344</v>
+        <v>4.378163482487345</v>
       </c>
       <c r="L2">
-        <v>0.4378163569022844</v>
+        <v>0.4378163569023265</v>
       </c>
       <c r="M2">
-        <v>4.378163482487168</v>
+        <v>4.378163482487091</v>
       </c>
       <c r="N2">
-        <v>0.9729578720439175</v>
+        <v>0.8440341447457987</v>
       </c>
       <c r="O2">
-        <v>0.7175004542770153</v>
+        <v>1.100000023840153</v>
       </c>
       <c r="P2">
-        <v>0.8439035640961189</v>
+        <v>0.9727947881380373</v>
       </c>
       <c r="Q2">
-        <v>17.56327454668237</v>
+        <v>31.7119228523478</v>
       </c>
       <c r="R2">
-        <v>-104.8932091443124</v>
+        <v>-89.99999999999653</v>
       </c>
       <c r="S2">
-        <v>151.7220699253674</v>
+        <v>137.5699449588465</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -3518,58 +3518,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1.020468705618021</v>
       </c>
       <c r="C3">
-        <v>1.10849935256055</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1.010036008422979</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>11.78335763776307</v>
       </c>
       <c r="F3">
-        <v>12.79984799194719</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>11.66289122708445</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>4.185910274912399</v>
+        <v>4.185910274912456</v>
       </c>
       <c r="I3">
-        <v>5.870495034006284</v>
+        <v>5.870495034005926</v>
       </c>
       <c r="J3">
-        <v>0.9578163680532483</v>
+        <v>0.9578163680481669</v>
       </c>
       <c r="K3">
-        <v>4.968163485641733</v>
+        <v>4.968163485594707</v>
       </c>
       <c r="L3">
-        <v>0.9578163680261339</v>
+        <v>0.9578163680263008</v>
       </c>
       <c r="M3">
-        <v>4.968163485594578</v>
+        <v>4.968163485594511</v>
       </c>
       <c r="N3">
-        <v>0.9653165427949276</v>
+        <v>0.8440065675549148</v>
       </c>
       <c r="O3">
-        <v>0.669786432244013</v>
+        <v>1.100000023840383</v>
       </c>
       <c r="P3">
-        <v>0.8518280946068217</v>
+        <v>0.9689144874145577</v>
       </c>
       <c r="Q3">
-        <v>16.29079354750229</v>
+        <v>31.98508613615191</v>
       </c>
       <c r="R3">
-        <v>-104.1338952714761</v>
+        <v>-89.99999999999645</v>
       </c>
       <c r="S3">
-        <v>153.6019224867848</v>
+        <v>137.6328508700616</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -3577,58 +3577,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.9013413882071819</v>
       </c>
       <c r="C4">
-        <v>1.040334427153928</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.9016673918744195</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>10.40779386226335</v>
       </c>
       <c r="F4">
-        <v>12.01274723129111</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>10.41155822836408</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>7.895175922947225</v>
+        <v>7.895175922947306</v>
       </c>
       <c r="I4">
-        <v>7.335082718453467</v>
+        <v>7.335082718453107</v>
       </c>
       <c r="J4">
-        <v>1.477816378918005</v>
+        <v>1.477816378913027</v>
       </c>
       <c r="K4">
-        <v>5.558163489027947</v>
+        <v>5.558163488980915</v>
       </c>
       <c r="L4">
-        <v>1.477816378890885</v>
+        <v>1.477816378891169</v>
       </c>
       <c r="M4">
-        <v>5.558163488980837</v>
+        <v>5.558163488980771</v>
       </c>
       <c r="N4">
-        <v>0.9579198071587197</v>
+        <v>0.8434715680207194</v>
       </c>
       <c r="O4">
-        <v>0.6279322069792089</v>
+        <v>1.100000023840569</v>
       </c>
       <c r="P4">
-        <v>0.8564846443872474</v>
+        <v>0.9656494086163243</v>
       </c>
       <c r="Q4">
-        <v>15.26462421738486</v>
+        <v>32.20512181945389</v>
       </c>
       <c r="R4">
-        <v>-103.4693739255812</v>
+        <v>-89.9999999999964</v>
       </c>
       <c r="S4">
-        <v>155.2583730680015</v>
+        <v>137.6537678120567</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -3636,58 +3636,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.9013413882071819</v>
       </c>
       <c r="C5">
-        <v>1.040334427153928</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.9016673918744195</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>10.40779386226335</v>
       </c>
       <c r="F5">
-        <v>12.01274723129111</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>10.41155822836408</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>7.895175922947224</v>
+        <v>7.895175922947299</v>
       </c>
       <c r="I5">
-        <v>7.335082718453457</v>
+        <v>7.335082718453101</v>
       </c>
       <c r="J5">
-        <v>1.477816378918004</v>
+        <v>1.477816378913028</v>
       </c>
       <c r="K5">
-        <v>5.558163489027946</v>
+        <v>5.558163488980913</v>
       </c>
       <c r="L5">
-        <v>1.477816378890884</v>
+        <v>1.477816378891169</v>
       </c>
       <c r="M5">
-        <v>5.558163488980837</v>
+        <v>5.558163488980769</v>
       </c>
       <c r="N5">
-        <v>0.9579198071587198</v>
+        <v>0.8434715680207194</v>
       </c>
       <c r="O5">
-        <v>0.627932206979209</v>
+        <v>1.100000023840569</v>
       </c>
       <c r="P5">
-        <v>0.8564846443872474</v>
+        <v>0.9656494086163243</v>
       </c>
       <c r="Q5">
-        <v>15.26462421738487</v>
+        <v>32.20512181945389</v>
       </c>
       <c r="R5">
-        <v>-103.4693739255812</v>
+        <v>-89.9999999999964</v>
       </c>
       <c r="S5">
-        <v>155.2583730680015</v>
+        <v>137.6537678120567</v>
       </c>
     </row>
   </sheetData>
@@ -3895,58 +3895,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1.170817013876365</v>
       </c>
       <c r="C2">
-        <v>1.170998762980853</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1.171492593911478</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>13.51943036266627</v>
       </c>
       <c r="F2">
-        <v>13.52152902055428</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>13.5272312889689</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.4428835862221404</v>
+        <v>0.4428835862221607</v>
       </c>
       <c r="I2">
-        <v>4.40271973851942</v>
+        <v>4.402719738519057</v>
       </c>
       <c r="J2">
-        <v>0.4378163569293868</v>
+        <v>0.437816356924225</v>
       </c>
       <c r="K2">
-        <v>4.378163482534344</v>
+        <v>4.378163482487345</v>
       </c>
       <c r="L2">
-        <v>0.4378163569022844</v>
+        <v>0.4378163569023265</v>
       </c>
       <c r="M2">
-        <v>4.378163482487168</v>
+        <v>4.378163482487091</v>
       </c>
       <c r="N2">
-        <v>0.9729578720439175</v>
+        <v>0.8440341447457987</v>
       </c>
       <c r="O2">
-        <v>0.7175004542770153</v>
+        <v>1.100000023840153</v>
       </c>
       <c r="P2">
-        <v>0.8439035640961189</v>
+        <v>0.9727947881380373</v>
       </c>
       <c r="Q2">
-        <v>17.56327454668237</v>
+        <v>31.7119228523478</v>
       </c>
       <c r="R2">
-        <v>-104.8932091443124</v>
+        <v>-89.99999999999653</v>
       </c>
       <c r="S2">
-        <v>151.7220699253674</v>
+        <v>137.5699449588465</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -3954,58 +3954,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1.020468705618021</v>
       </c>
       <c r="C3">
-        <v>1.10849935256055</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1.010036008422979</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>11.78335763776307</v>
       </c>
       <c r="F3">
-        <v>12.79984799194719</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>11.66289122708445</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>4.185910274912399</v>
+        <v>4.185910274912456</v>
       </c>
       <c r="I3">
-        <v>5.870495034006284</v>
+        <v>5.870495034005926</v>
       </c>
       <c r="J3">
-        <v>0.9578163680532483</v>
+        <v>0.9578163680481669</v>
       </c>
       <c r="K3">
-        <v>4.968163485641733</v>
+        <v>4.968163485594707</v>
       </c>
       <c r="L3">
-        <v>0.9578163680261339</v>
+        <v>0.9578163680263008</v>
       </c>
       <c r="M3">
-        <v>4.968163485594578</v>
+        <v>4.968163485594511</v>
       </c>
       <c r="N3">
-        <v>0.9653165427949276</v>
+        <v>0.8440065675549148</v>
       </c>
       <c r="O3">
-        <v>0.669786432244013</v>
+        <v>1.100000023840383</v>
       </c>
       <c r="P3">
-        <v>0.8518280946068217</v>
+        <v>0.9689144874145577</v>
       </c>
       <c r="Q3">
-        <v>16.29079354750229</v>
+        <v>31.98508613615191</v>
       </c>
       <c r="R3">
-        <v>-104.1338952714761</v>
+        <v>-89.99999999999645</v>
       </c>
       <c r="S3">
-        <v>153.6019224867848</v>
+        <v>137.6328508700616</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -4013,58 +4013,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.9013413882071819</v>
       </c>
       <c r="C4">
-        <v>1.040334427153928</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.9016673918744195</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>10.40779386226335</v>
       </c>
       <c r="F4">
-        <v>12.01274723129111</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>10.41155822836408</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>7.895175922947225</v>
+        <v>7.895175922947306</v>
       </c>
       <c r="I4">
-        <v>7.335082718453467</v>
+        <v>7.335082718453107</v>
       </c>
       <c r="J4">
-        <v>1.477816378918005</v>
+        <v>1.477816378913027</v>
       </c>
       <c r="K4">
-        <v>5.558163489027947</v>
+        <v>5.558163488980915</v>
       </c>
       <c r="L4">
-        <v>1.477816378890885</v>
+        <v>1.477816378891169</v>
       </c>
       <c r="M4">
-        <v>5.558163488980837</v>
+        <v>5.558163488980771</v>
       </c>
       <c r="N4">
-        <v>0.9579198071587197</v>
+        <v>0.8434715680207194</v>
       </c>
       <c r="O4">
-        <v>0.6279322069792089</v>
+        <v>1.100000023840569</v>
       </c>
       <c r="P4">
-        <v>0.8564846443872474</v>
+        <v>0.9656494086163243</v>
       </c>
       <c r="Q4">
-        <v>15.26462421738486</v>
+        <v>32.20512181945389</v>
       </c>
       <c r="R4">
-        <v>-103.4693739255812</v>
+        <v>-89.9999999999964</v>
       </c>
       <c r="S4">
-        <v>155.2583730680015</v>
+        <v>137.6537678120567</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -4072,58 +4072,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.9013413882071819</v>
       </c>
       <c r="C5">
-        <v>1.040334427153928</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.9016673918744195</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>10.40779386226335</v>
       </c>
       <c r="F5">
-        <v>12.01274723129111</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>10.41155822836408</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>7.895175922947224</v>
+        <v>7.895175922947299</v>
       </c>
       <c r="I5">
-        <v>7.335082718453457</v>
+        <v>7.335082718453101</v>
       </c>
       <c r="J5">
-        <v>1.477816378918004</v>
+        <v>1.477816378913028</v>
       </c>
       <c r="K5">
-        <v>5.558163489027946</v>
+        <v>5.558163488980913</v>
       </c>
       <c r="L5">
-        <v>1.477816378890884</v>
+        <v>1.477816378891169</v>
       </c>
       <c r="M5">
-        <v>5.558163488980837</v>
+        <v>5.558163488980769</v>
       </c>
       <c r="N5">
-        <v>0.9579198071587198</v>
+        <v>0.8434715680207194</v>
       </c>
       <c r="O5">
-        <v>0.627932206979209</v>
+        <v>1.100000023840569</v>
       </c>
       <c r="P5">
-        <v>0.8564846443872474</v>
+        <v>0.9656494086163243</v>
       </c>
       <c r="Q5">
-        <v>15.26462421738487</v>
+        <v>32.20512181945389</v>
       </c>
       <c r="R5">
-        <v>-103.4693739255812</v>
+        <v>-89.9999999999964</v>
       </c>
       <c r="S5">
-        <v>155.2583730680015</v>
+        <v>137.6537678120567</v>
       </c>
     </row>
   </sheetData>
@@ -4203,58 +4203,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2.304451709204056</v>
       </c>
       <c r="C2">
-        <v>2.307394468727928</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>2.306476761395013</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>26.6095162928691</v>
       </c>
       <c r="F2">
-        <v>26.64349635293446</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>26.63289958142054</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.5041743431842544</v>
+        <v>0.5041743431842567</v>
       </c>
       <c r="I2">
-        <v>5.006897135806584</v>
+        <v>5.006897135806157</v>
       </c>
       <c r="J2">
-        <v>0.4975185876946874</v>
+        <v>0.4975185876920994</v>
       </c>
       <c r="K2">
-        <v>4.975185775457811</v>
+        <v>4.975185775488431</v>
       </c>
       <c r="L2">
-        <v>0.4975185877124232</v>
+        <v>0.497518587712459</v>
       </c>
       <c r="M2">
-        <v>4.975185775488254</v>
+        <v>4.97518577548815</v>
       </c>
       <c r="N2">
-        <v>0.5785850458643943</v>
+        <v>0.5778549958900403</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>0.9999999999962847</v>
       </c>
       <c r="P2">
-        <v>0.5785850458648649</v>
+        <v>0.5780849144276639</v>
       </c>
       <c r="Q2">
-        <v>-0.01310313119137088</v>
+        <v>59.88716006626888</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>-89.99999999999636</v>
       </c>
       <c r="S2">
-        <v>179.9868968685288</v>
+        <v>120.0996242896476</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -4262,58 +4262,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1.684845595525955</v>
       </c>
       <c r="C3">
-        <v>2.144785402460348</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1.543474101037902</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>19.45492116239731</v>
       </c>
       <c r="F3">
-        <v>24.76584858928923</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>17.82250375442897</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>7.698542227644789</v>
+        <v>7.698542227644828</v>
       </c>
       <c r="I3">
-        <v>6.432196710719398</v>
+        <v>6.432196710718991</v>
       </c>
       <c r="J3">
-        <v>1.495918608642645</v>
+        <v>1.495918608640806</v>
       </c>
       <c r="K3">
-        <v>5.565185778068525</v>
+        <v>5.565185778099434</v>
       </c>
       <c r="L3">
-        <v>1.495918608660561</v>
+        <v>1.495918608660816</v>
       </c>
       <c r="M3">
-        <v>5.565185778099361</v>
+        <v>5.565185778099255</v>
       </c>
       <c r="N3">
-        <v>0.6950234972340792</v>
+        <v>0.5407731743511122</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>0.9999999999980868</v>
       </c>
       <c r="P3">
-        <v>0.6950234972340121</v>
+        <v>0.7514492206972073</v>
       </c>
       <c r="Q3">
-        <v>-7.611827049086783</v>
+        <v>42.2903649473445</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>-89.99999999999652</v>
       </c>
       <c r="S3">
-        <v>172.3881729507654</v>
+        <v>122.1643601284607</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -4321,58 +4321,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1.224899235816899</v>
       </c>
       <c r="C4">
-        <v>1.791382665021896</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1.312244351459671</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>14.14391807058107</v>
       </c>
       <c r="F4">
-        <v>20.68510527744042</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>15.15249259115614</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>14.8217784003751</v>
+        <v>14.82177840037519</v>
       </c>
       <c r="I4">
-        <v>7.872438169825732</v>
+        <v>7.872438169825329</v>
       </c>
       <c r="J4">
-        <v>2.494318629322498</v>
+        <v>2.494318629320983</v>
       </c>
       <c r="K4">
-        <v>6.155185781258161</v>
+        <v>6.155185781289128</v>
       </c>
       <c r="L4">
-        <v>2.494318629340454</v>
+        <v>2.494318629340928</v>
       </c>
       <c r="M4">
-        <v>6.155185781289154</v>
+        <v>6.155185781289043</v>
       </c>
       <c r="N4">
-        <v>0.7474500608991325</v>
+        <v>0.5992308608385498</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>0.9999999999990241</v>
       </c>
       <c r="P4">
-        <v>0.7474500608986431</v>
+        <v>0.8180273553921663</v>
       </c>
       <c r="Q4">
-        <v>-6.297561754805892</v>
+        <v>35.14600558028982</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>-89.99999999999639</v>
       </c>
       <c r="S4">
-        <v>173.702438245086</v>
+        <v>126.7970300907754</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -4380,58 +4380,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1.224899235816899</v>
       </c>
       <c r="C5">
-        <v>1.791382665021898</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>1.31224435145967</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>14.14391807058107</v>
       </c>
       <c r="F5">
-        <v>20.68510527744045</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>15.15249259115612</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>14.82177840037509</v>
+        <v>14.82177840037519</v>
       </c>
       <c r="I5">
-        <v>7.872438169825724</v>
+        <v>7.872438169825323</v>
       </c>
       <c r="J5">
-        <v>2.494318629322495</v>
+        <v>2.494318629320986</v>
       </c>
       <c r="K5">
-        <v>6.155185781258152</v>
+        <v>6.155185781289128</v>
       </c>
       <c r="L5">
-        <v>2.494318629340448</v>
+        <v>2.494318629340926</v>
       </c>
       <c r="M5">
-        <v>6.15518578128915</v>
+        <v>6.155185781289043</v>
       </c>
       <c r="N5">
-        <v>0.7474500608991327</v>
+        <v>0.5992308608385494</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>0.9999999999990241</v>
       </c>
       <c r="P5">
-        <v>0.7474500608986436</v>
+        <v>0.8180273553921662</v>
       </c>
       <c r="Q5">
-        <v>-6.297561754805924</v>
+        <v>35.14600558028984</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>-89.99999999999639</v>
       </c>
       <c r="S5">
-        <v>173.702438245086</v>
+        <v>126.7970300907753</v>
       </c>
     </row>
   </sheetData>
@@ -4511,58 +4511,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2.304451709204056</v>
       </c>
       <c r="C2">
-        <v>2.307394468727928</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>2.306476761395013</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>26.6095162928691</v>
       </c>
       <c r="F2">
-        <v>26.64349635293446</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>26.63289958142054</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.5041743431842544</v>
+        <v>0.5041743431842567</v>
       </c>
       <c r="I2">
-        <v>5.006897135806584</v>
+        <v>5.006897135806157</v>
       </c>
       <c r="J2">
-        <v>0.4975185876946874</v>
+        <v>0.4975185876920994</v>
       </c>
       <c r="K2">
-        <v>4.975185775457811</v>
+        <v>4.975185775488431</v>
       </c>
       <c r="L2">
-        <v>0.4975185877124232</v>
+        <v>0.497518587712459</v>
       </c>
       <c r="M2">
-        <v>4.975185775488254</v>
+        <v>4.97518577548815</v>
       </c>
       <c r="N2">
-        <v>0.5785850458643943</v>
+        <v>0.5778549958900403</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>0.9999999999962847</v>
       </c>
       <c r="P2">
-        <v>0.5785850458648649</v>
+        <v>0.5780849144276639</v>
       </c>
       <c r="Q2">
-        <v>-0.01310313119137088</v>
+        <v>59.88716006626888</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>-89.99999999999636</v>
       </c>
       <c r="S2">
-        <v>179.9868968685288</v>
+        <v>120.0996242896476</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -4570,58 +4570,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1.684845595525955</v>
       </c>
       <c r="C3">
-        <v>2.144785402460348</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1.543474101037902</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>19.45492116239731</v>
       </c>
       <c r="F3">
-        <v>24.76584858928923</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>17.82250375442897</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>7.698542227644789</v>
+        <v>7.698542227644828</v>
       </c>
       <c r="I3">
-        <v>6.432196710719398</v>
+        <v>6.432196710718991</v>
       </c>
       <c r="J3">
-        <v>1.495918608642645</v>
+        <v>1.495918608640806</v>
       </c>
       <c r="K3">
-        <v>5.565185778068525</v>
+        <v>5.565185778099434</v>
       </c>
       <c r="L3">
-        <v>1.495918608660561</v>
+        <v>1.495918608660816</v>
       </c>
       <c r="M3">
-        <v>5.565185778099361</v>
+        <v>5.565185778099255</v>
       </c>
       <c r="N3">
-        <v>0.6950234972340792</v>
+        <v>0.5407731743511122</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>0.9999999999980868</v>
       </c>
       <c r="P3">
-        <v>0.6950234972340121</v>
+        <v>0.7514492206972073</v>
       </c>
       <c r="Q3">
-        <v>-7.611827049086783</v>
+        <v>42.2903649473445</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>-89.99999999999652</v>
       </c>
       <c r="S3">
-        <v>172.3881729507654</v>
+        <v>122.1643601284607</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -4629,58 +4629,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1.224899235816899</v>
       </c>
       <c r="C4">
-        <v>1.791382665021896</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1.312244351459671</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>14.14391807058107</v>
       </c>
       <c r="F4">
-        <v>20.68510527744042</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>15.15249259115614</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>14.8217784003751</v>
+        <v>14.82177840037519</v>
       </c>
       <c r="I4">
-        <v>7.872438169825732</v>
+        <v>7.872438169825329</v>
       </c>
       <c r="J4">
-        <v>2.494318629322498</v>
+        <v>2.494318629320983</v>
       </c>
       <c r="K4">
-        <v>6.155185781258161</v>
+        <v>6.155185781289128</v>
       </c>
       <c r="L4">
-        <v>2.494318629340454</v>
+        <v>2.494318629340928</v>
       </c>
       <c r="M4">
-        <v>6.155185781289154</v>
+        <v>6.155185781289043</v>
       </c>
       <c r="N4">
-        <v>0.7474500608991325</v>
+        <v>0.5992308608385498</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>0.9999999999990241</v>
       </c>
       <c r="P4">
-        <v>0.7474500608986431</v>
+        <v>0.8180273553921663</v>
       </c>
       <c r="Q4">
-        <v>-6.297561754805892</v>
+        <v>35.14600558028982</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>-89.99999999999639</v>
       </c>
       <c r="S4">
-        <v>173.702438245086</v>
+        <v>126.7970300907754</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -4688,58 +4688,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1.224899235816899</v>
       </c>
       <c r="C5">
-        <v>1.791382665021898</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>1.31224435145967</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>14.14391807058107</v>
       </c>
       <c r="F5">
-        <v>20.68510527744045</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>15.15249259115612</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>14.82177840037509</v>
+        <v>14.82177840037519</v>
       </c>
       <c r="I5">
-        <v>7.872438169825724</v>
+        <v>7.872438169825323</v>
       </c>
       <c r="J5">
-        <v>2.494318629322495</v>
+        <v>2.494318629320986</v>
       </c>
       <c r="K5">
-        <v>6.155185781258152</v>
+        <v>6.155185781289128</v>
       </c>
       <c r="L5">
-        <v>2.494318629340448</v>
+        <v>2.494318629340926</v>
       </c>
       <c r="M5">
-        <v>6.15518578128915</v>
+        <v>6.155185781289043</v>
       </c>
       <c r="N5">
-        <v>0.7474500608991327</v>
+        <v>0.5992308608385494</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>0.9999999999990241</v>
       </c>
       <c r="P5">
-        <v>0.7474500608986436</v>
+        <v>0.8180273553921662</v>
       </c>
       <c r="Q5">
-        <v>-6.297561754805924</v>
+        <v>35.14600558028984</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>-89.99999999999639</v>
       </c>
       <c r="S5">
-        <v>173.702438245086</v>
+        <v>126.7970300907753</v>
       </c>
     </row>
   </sheetData>
@@ -4819,58 +4819,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1.012885714576425</v>
       </c>
       <c r="C2">
-        <v>1.013102923845676</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1.013588406235421</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>11.69579679938051</v>
       </c>
       <c r="F2">
-        <v>11.69830491598196</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>11.70391078375008</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.5041743431842544</v>
+        <v>0.5041743431842567</v>
       </c>
       <c r="I2">
-        <v>5.006897135806584</v>
+        <v>5.006897135806157</v>
       </c>
       <c r="J2">
-        <v>0.4975185876946874</v>
+        <v>0.4975185876920994</v>
       </c>
       <c r="K2">
-        <v>4.975185775457811</v>
+        <v>4.975185775488431</v>
       </c>
       <c r="L2">
-        <v>0.4975185877124232</v>
+        <v>0.497518587712459</v>
       </c>
       <c r="M2">
-        <v>4.975185775488254</v>
+        <v>4.97518577548815</v>
       </c>
       <c r="N2">
-        <v>0.8721332518534242</v>
+        <v>0.7492067188226383</v>
       </c>
       <c r="O2">
-        <v>0.6208257825095037</v>
+        <v>0.9999999999987974</v>
       </c>
       <c r="P2">
-        <v>0.7490594668689452</v>
+        <v>0.8719401990676209</v>
       </c>
       <c r="Q2">
-        <v>16.55576890986408</v>
+        <v>32.31584613269226</v>
       </c>
       <c r="R2">
-        <v>-106.1399873258002</v>
+        <v>-89.99999999999655</v>
       </c>
       <c r="S2">
-        <v>152.3303371030605</v>
+        <v>136.5651455806771</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -4878,58 +4878,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.8351922431613388</v>
       </c>
       <c r="C3">
-        <v>0.9576169384185383</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.8150213495726398</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>9.643969328285728</v>
       </c>
       <c r="F3">
-        <v>11.05760794352977</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>9.411055911421114</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>7.698542227644789</v>
+        <v>7.698542227644828</v>
       </c>
       <c r="I3">
-        <v>6.432196710719398</v>
+        <v>6.432196710718991</v>
       </c>
       <c r="J3">
-        <v>1.495918608642645</v>
+        <v>1.495918608640806</v>
       </c>
       <c r="K3">
-        <v>5.565185778068525</v>
+        <v>5.565185778099434</v>
       </c>
       <c r="L3">
-        <v>1.495918608660561</v>
+        <v>1.495918608660816</v>
       </c>
       <c r="M3">
-        <v>5.565185778099361</v>
+        <v>5.565185778099255</v>
       </c>
       <c r="N3">
-        <v>0.8671834304540896</v>
+        <v>0.7615594742962095</v>
       </c>
       <c r="O3">
-        <v>0.5701359740030982</v>
+        <v>0.9999999999991965</v>
       </c>
       <c r="P3">
-        <v>0.7780446838807024</v>
+        <v>0.877371251159636</v>
       </c>
       <c r="Q3">
-        <v>15.07716951670869</v>
+        <v>32.13594383429049</v>
       </c>
       <c r="R3">
-        <v>-103.4150584572222</v>
+        <v>-89.99999999999645</v>
       </c>
       <c r="S3">
-        <v>154.9843720112472</v>
+        <v>137.3083573823813</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -4937,58 +4937,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.6999120446284219</v>
       </c>
       <c r="C4">
-        <v>0.8779780941084492</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.7099194197390576</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>8.081888147505616</v>
       </c>
       <c r="F4">
-        <v>10.13801777952216</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>8.197443361785757</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>14.8217784003751</v>
+        <v>14.82177840037519</v>
       </c>
       <c r="I4">
-        <v>7.872438169825732</v>
+        <v>7.872438169825329</v>
       </c>
       <c r="J4">
-        <v>2.494318629322498</v>
+        <v>2.494318629320983</v>
       </c>
       <c r="K4">
-        <v>6.155185781258161</v>
+        <v>6.155185781289128</v>
       </c>
       <c r="L4">
-        <v>2.494318629340454</v>
+        <v>2.494318629340928</v>
       </c>
       <c r="M4">
-        <v>6.155185781289154</v>
+        <v>6.155185781289043</v>
       </c>
       <c r="N4">
-        <v>0.8595183170292721</v>
+        <v>0.7700746676618133</v>
       </c>
       <c r="O4">
-        <v>0.526165712950652</v>
+        <v>0.999999999999447</v>
       </c>
       <c r="P4">
-        <v>0.793440478635774</v>
+        <v>0.8785874061674938</v>
       </c>
       <c r="Q4">
-        <v>14.16121021104031</v>
+        <v>32.21715262800947</v>
       </c>
       <c r="R4">
-        <v>-101.1058570224848</v>
+        <v>-89.99999999999638</v>
       </c>
       <c r="S4">
-        <v>157.3127817016637</v>
+        <v>137.8628958470784</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -4996,58 +4996,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.699912044628422</v>
       </c>
       <c r="C5">
-        <v>0.8779780941084497</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.7099194197390573</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>8.081888147505618</v>
       </c>
       <c r="F5">
-        <v>10.13801777952216</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>8.197443361785753</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>14.82177840037509</v>
+        <v>14.82177840037519</v>
       </c>
       <c r="I5">
-        <v>7.872438169825724</v>
+        <v>7.872438169825323</v>
       </c>
       <c r="J5">
-        <v>2.494318629322495</v>
+        <v>2.494318629320986</v>
       </c>
       <c r="K5">
-        <v>6.155185781258152</v>
+        <v>6.155185781289128</v>
       </c>
       <c r="L5">
-        <v>2.494318629340448</v>
+        <v>2.494318629340926</v>
       </c>
       <c r="M5">
-        <v>6.15518578128915</v>
+        <v>6.155185781289043</v>
       </c>
       <c r="N5">
-        <v>0.8595183170292721</v>
+        <v>0.7700746676618129</v>
       </c>
       <c r="O5">
-        <v>0.526165712950652</v>
+        <v>0.9999999999994468</v>
       </c>
       <c r="P5">
-        <v>0.793440478635774</v>
+        <v>0.8785874061674938</v>
       </c>
       <c r="Q5">
-        <v>14.1612102110403</v>
+        <v>32.21715262800947</v>
       </c>
       <c r="R5">
-        <v>-101.1058570224848</v>
+        <v>-89.99999999999636</v>
       </c>
       <c r="S5">
-        <v>157.3127817016637</v>
+        <v>137.8628958470784</v>
       </c>
     </row>
   </sheetData>
@@ -5127,58 +5127,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1.012885714576425</v>
       </c>
       <c r="C2">
-        <v>1.013102923845676</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1.013588406235421</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>11.69579679938051</v>
       </c>
       <c r="F2">
-        <v>11.69830491598196</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>11.70391078375008</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.5041743431842544</v>
+        <v>0.5041743431842567</v>
       </c>
       <c r="I2">
-        <v>5.006897135806584</v>
+        <v>5.006897135806157</v>
       </c>
       <c r="J2">
-        <v>0.4975185876946874</v>
+        <v>0.4975185876920994</v>
       </c>
       <c r="K2">
-        <v>4.975185775457811</v>
+        <v>4.975185775488431</v>
       </c>
       <c r="L2">
-        <v>0.4975185877124232</v>
+        <v>0.497518587712459</v>
       </c>
       <c r="M2">
-        <v>4.975185775488254</v>
+        <v>4.97518577548815</v>
       </c>
       <c r="N2">
-        <v>0.8721332518534242</v>
+        <v>0.7492067188226383</v>
       </c>
       <c r="O2">
-        <v>0.6208257825095037</v>
+        <v>0.9999999999987974</v>
       </c>
       <c r="P2">
-        <v>0.7490594668689452</v>
+        <v>0.8719401990676209</v>
       </c>
       <c r="Q2">
-        <v>16.55576890986408</v>
+        <v>32.31584613269226</v>
       </c>
       <c r="R2">
-        <v>-106.1399873258002</v>
+        <v>-89.99999999999655</v>
       </c>
       <c r="S2">
-        <v>152.3303371030605</v>
+        <v>136.5651455806771</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -5186,58 +5186,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.8351922431613388</v>
       </c>
       <c r="C3">
-        <v>0.9576169384185383</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.8150213495726398</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>9.643969328285728</v>
       </c>
       <c r="F3">
-        <v>11.05760794352977</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>9.411055911421114</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>7.698542227644789</v>
+        <v>7.698542227644828</v>
       </c>
       <c r="I3">
-        <v>6.432196710719398</v>
+        <v>6.432196710718991</v>
       </c>
       <c r="J3">
-        <v>1.495918608642645</v>
+        <v>1.495918608640806</v>
       </c>
       <c r="K3">
-        <v>5.565185778068525</v>
+        <v>5.565185778099434</v>
       </c>
       <c r="L3">
-        <v>1.495918608660561</v>
+        <v>1.495918608660816</v>
       </c>
       <c r="M3">
-        <v>5.565185778099361</v>
+        <v>5.565185778099255</v>
       </c>
       <c r="N3">
-        <v>0.8671834304540896</v>
+        <v>0.7615594742962095</v>
       </c>
       <c r="O3">
-        <v>0.5701359740030982</v>
+        <v>0.9999999999991965</v>
       </c>
       <c r="P3">
-        <v>0.7780446838807024</v>
+        <v>0.877371251159636</v>
       </c>
       <c r="Q3">
-        <v>15.07716951670869</v>
+        <v>32.13594383429049</v>
       </c>
       <c r="R3">
-        <v>-103.4150584572222</v>
+        <v>-89.99999999999645</v>
       </c>
       <c r="S3">
-        <v>154.9843720112472</v>
+        <v>137.3083573823813</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -5245,58 +5245,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.6999120446284219</v>
       </c>
       <c r="C4">
-        <v>0.8779780941084492</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.7099194197390576</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>8.081888147505616</v>
       </c>
       <c r="F4">
-        <v>10.13801777952216</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>8.197443361785757</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>14.8217784003751</v>
+        <v>14.82177840037519</v>
       </c>
       <c r="I4">
-        <v>7.872438169825732</v>
+        <v>7.872438169825329</v>
       </c>
       <c r="J4">
-        <v>2.494318629322498</v>
+        <v>2.494318629320983</v>
       </c>
       <c r="K4">
-        <v>6.155185781258161</v>
+        <v>6.155185781289128</v>
       </c>
       <c r="L4">
-        <v>2.494318629340454</v>
+        <v>2.494318629340928</v>
       </c>
       <c r="M4">
-        <v>6.155185781289154</v>
+        <v>6.155185781289043</v>
       </c>
       <c r="N4">
-        <v>0.8595183170292721</v>
+        <v>0.7700746676618133</v>
       </c>
       <c r="O4">
-        <v>0.526165712950652</v>
+        <v>0.999999999999447</v>
       </c>
       <c r="P4">
-        <v>0.793440478635774</v>
+        <v>0.8785874061674938</v>
       </c>
       <c r="Q4">
-        <v>14.16121021104031</v>
+        <v>32.21715262800947</v>
       </c>
       <c r="R4">
-        <v>-101.1058570224848</v>
+        <v>-89.99999999999638</v>
       </c>
       <c r="S4">
-        <v>157.3127817016637</v>
+        <v>137.8628958470784</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -5304,58 +5304,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.699912044628422</v>
       </c>
       <c r="C5">
-        <v>0.8779780941084497</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.7099194197390573</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>8.081888147505618</v>
       </c>
       <c r="F5">
-        <v>10.13801777952216</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>8.197443361785753</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>14.82177840037509</v>
+        <v>14.82177840037519</v>
       </c>
       <c r="I5">
-        <v>7.872438169825724</v>
+        <v>7.872438169825323</v>
       </c>
       <c r="J5">
-        <v>2.494318629322495</v>
+        <v>2.494318629320986</v>
       </c>
       <c r="K5">
-        <v>6.155185781258152</v>
+        <v>6.155185781289128</v>
       </c>
       <c r="L5">
-        <v>2.494318629340448</v>
+        <v>2.494318629340926</v>
       </c>
       <c r="M5">
-        <v>6.15518578128915</v>
+        <v>6.155185781289043</v>
       </c>
       <c r="N5">
-        <v>0.8595183170292721</v>
+        <v>0.7700746676618129</v>
       </c>
       <c r="O5">
-        <v>0.526165712950652</v>
+        <v>0.9999999999994468</v>
       </c>
       <c r="P5">
-        <v>0.793440478635774</v>
+        <v>0.8785874061674938</v>
       </c>
       <c r="Q5">
-        <v>14.1612102110403</v>
+        <v>32.21715262800947</v>
       </c>
       <c r="R5">
-        <v>-101.1058570224848</v>
+        <v>-89.99999999999636</v>
       </c>
       <c r="S5">
-        <v>157.3127817016637</v>
+        <v>137.8628958470784</v>
       </c>
     </row>
   </sheetData>
@@ -5435,58 +5435,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>2.881307834727568</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2.884527493204643</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2.883549636712145</v>
       </c>
       <c r="E2">
-        <v>33.27047707996278</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>33.30765449373155</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>33.29636317954809</v>
       </c>
       <c r="H2">
-        <v>0.4428835862221607</v>
+        <v>0.4428835862221404</v>
       </c>
       <c r="I2">
-        <v>4.402719738519057</v>
+        <v>4.40271973851942</v>
       </c>
       <c r="J2">
-        <v>0.437816356924225</v>
+        <v>0.4378163569293868</v>
       </c>
       <c r="K2">
-        <v>4.378163482487345</v>
+        <v>4.378163482534344</v>
       </c>
       <c r="L2">
-        <v>0.4378163569023265</v>
+        <v>0.4378163569022844</v>
       </c>
       <c r="M2">
-        <v>4.378163482487091</v>
+        <v>4.378163482487168</v>
       </c>
       <c r="N2">
-        <v>0.6355772023502927</v>
+        <v>0.636280712791619</v>
       </c>
       <c r="O2">
-        <v>1.1000000238379</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0.6357927364583869</v>
+        <v>0.6362807127881797</v>
       </c>
       <c r="Q2">
-        <v>59.90088731360098</v>
+        <v>-0.01117384664767678</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999633</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>120.0878544346237</v>
+        <v>179.9888261535143</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -5494,58 +5494,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>2.248943182936928</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2.659777356923221</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>2.088302030918968</v>
       </c>
       <c r="E3">
-        <v>25.96855904121619</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>30.71246346008186</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>24.11363479400617</v>
       </c>
       <c r="H3">
-        <v>4.185910274912456</v>
+        <v>4.185910274912399</v>
       </c>
       <c r="I3">
-        <v>5.870495034005926</v>
+        <v>5.870495034006284</v>
       </c>
       <c r="J3">
-        <v>0.9578163680481669</v>
+        <v>0.9578163680532483</v>
       </c>
       <c r="K3">
-        <v>4.968163485594707</v>
+        <v>4.968163485641733</v>
       </c>
       <c r="L3">
-        <v>0.9578163680263008</v>
+        <v>0.9578163680261339</v>
       </c>
       <c r="M3">
-        <v>4.968163485594511</v>
+        <v>4.968163485594578</v>
       </c>
       <c r="N3">
-        <v>0.5967063269904345</v>
+        <v>0.7178088853018512</v>
       </c>
       <c r="O3">
-        <v>1.100000023838578</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>0.7599982922815229</v>
+        <v>0.7178088852998012</v>
       </c>
       <c r="Q3">
-        <v>48.84809195671546</v>
+        <v>-6.313450644998808</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999643</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>121.109045449341</v>
+        <v>173.6865493550667</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -5553,58 +5553,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>1.780157175146007</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>2.314120905097126</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1.728412445116583</v>
       </c>
       <c r="E4">
-        <v>20.55548448540782</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>26.72116654990332</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>19.95798780917517</v>
       </c>
       <c r="H4">
-        <v>7.895175922947306</v>
+        <v>7.895175922947225</v>
       </c>
       <c r="I4">
-        <v>7.335082718453107</v>
+        <v>7.335082718453467</v>
       </c>
       <c r="J4">
-        <v>1.477816378913027</v>
+        <v>1.477816378918005</v>
       </c>
       <c r="K4">
-        <v>5.558163488980915</v>
+        <v>5.558163489027947</v>
       </c>
       <c r="L4">
-        <v>1.477816378891169</v>
+        <v>1.477816378890885</v>
       </c>
       <c r="M4">
-        <v>5.558163488980771</v>
+        <v>5.558163488980837</v>
       </c>
       <c r="N4">
-        <v>0.6175627786591105</v>
+        <v>0.7719945678108373</v>
       </c>
       <c r="O4">
-        <v>1.100000023839263</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>0.826836754355374</v>
+        <v>0.7719945678096874</v>
       </c>
       <c r="Q4">
-        <v>41.92164926482276</v>
+        <v>-6.619958059522241</v>
       </c>
       <c r="R4">
-        <v>-89.9999999999964</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>123.7614475143174</v>
+        <v>173.3800419405132</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -5612,58 +5612,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>1.780157175146008</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>2.314120905097127</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1.728412445116581</v>
       </c>
       <c r="E5">
-        <v>20.55548448540783</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>26.72116654990333</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>19.95798780917515</v>
       </c>
       <c r="H5">
-        <v>7.895175922947299</v>
+        <v>7.895175922947224</v>
       </c>
       <c r="I5">
-        <v>7.335082718453101</v>
+        <v>7.335082718453457</v>
       </c>
       <c r="J5">
-        <v>1.477816378913028</v>
+        <v>1.477816378918004</v>
       </c>
       <c r="K5">
-        <v>5.558163488980913</v>
+        <v>5.558163489027946</v>
       </c>
       <c r="L5">
-        <v>1.477816378891169</v>
+        <v>1.477816378890884</v>
       </c>
       <c r="M5">
-        <v>5.558163488980769</v>
+        <v>5.558163488980837</v>
       </c>
       <c r="N5">
-        <v>0.6175627786591099</v>
+        <v>0.7719945678108373</v>
       </c>
       <c r="O5">
-        <v>1.100000023839263</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>0.8268367543553737</v>
+        <v>0.7719945678096877</v>
       </c>
       <c r="Q5">
-        <v>41.92164926482278</v>
+        <v>-6.619958059522241</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999639</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>123.7614475143174</v>
+        <v>173.3800419405131</v>
       </c>
     </row>
   </sheetData>
@@ -5743,58 +5743,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>2.881307834727568</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2.884527493204643</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2.883549636712145</v>
       </c>
       <c r="E2">
-        <v>33.27047707996278</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>33.30765449373155</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>33.29636317954809</v>
       </c>
       <c r="H2">
-        <v>0.4428835862221607</v>
+        <v>0.4428835862221404</v>
       </c>
       <c r="I2">
-        <v>4.402719738519057</v>
+        <v>4.40271973851942</v>
       </c>
       <c r="J2">
-        <v>0.437816356924225</v>
+        <v>0.4378163569293868</v>
       </c>
       <c r="K2">
-        <v>4.378163482487345</v>
+        <v>4.378163482534344</v>
       </c>
       <c r="L2">
-        <v>0.4378163569023265</v>
+        <v>0.4378163569022844</v>
       </c>
       <c r="M2">
-        <v>4.378163482487091</v>
+        <v>4.378163482487168</v>
       </c>
       <c r="N2">
-        <v>0.6355772023502927</v>
+        <v>0.636280712791619</v>
       </c>
       <c r="O2">
-        <v>1.1000000238379</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0.6357927364583869</v>
+        <v>0.6362807127881797</v>
       </c>
       <c r="Q2">
-        <v>59.90088731360098</v>
+        <v>-0.01117384664767678</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999633</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>120.0878544346237</v>
+        <v>179.9888261535143</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -5802,58 +5802,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>2.248943182936928</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2.659777356923221</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>2.088302030918968</v>
       </c>
       <c r="E3">
-        <v>25.96855904121619</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>30.71246346008186</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>24.11363479400617</v>
       </c>
       <c r="H3">
-        <v>4.185910274912456</v>
+        <v>4.185910274912399</v>
       </c>
       <c r="I3">
-        <v>5.870495034005926</v>
+        <v>5.870495034006284</v>
       </c>
       <c r="J3">
-        <v>0.9578163680481669</v>
+        <v>0.9578163680532483</v>
       </c>
       <c r="K3">
-        <v>4.968163485594707</v>
+        <v>4.968163485641733</v>
       </c>
       <c r="L3">
-        <v>0.9578163680263008</v>
+        <v>0.9578163680261339</v>
       </c>
       <c r="M3">
-        <v>4.968163485594511</v>
+        <v>4.968163485594578</v>
       </c>
       <c r="N3">
-        <v>0.5967063269904345</v>
+        <v>0.7178088853018512</v>
       </c>
       <c r="O3">
-        <v>1.100000023838578</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>0.7599982922815229</v>
+        <v>0.7178088852998012</v>
       </c>
       <c r="Q3">
-        <v>48.84809195671546</v>
+        <v>-6.313450644998808</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999643</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>121.109045449341</v>
+        <v>173.6865493550667</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -5861,58 +5861,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>1.780157175146007</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>2.314120905097126</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1.728412445116583</v>
       </c>
       <c r="E4">
-        <v>20.55548448540782</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>26.72116654990332</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>19.95798780917517</v>
       </c>
       <c r="H4">
-        <v>7.895175922947306</v>
+        <v>7.895175922947225</v>
       </c>
       <c r="I4">
-        <v>7.335082718453107</v>
+        <v>7.335082718453467</v>
       </c>
       <c r="J4">
-        <v>1.477816378913027</v>
+        <v>1.477816378918005</v>
       </c>
       <c r="K4">
-        <v>5.558163488980915</v>
+        <v>5.558163489027947</v>
       </c>
       <c r="L4">
-        <v>1.477816378891169</v>
+        <v>1.477816378890885</v>
       </c>
       <c r="M4">
-        <v>5.558163488980771</v>
+        <v>5.558163488980837</v>
       </c>
       <c r="N4">
-        <v>0.6175627786591105</v>
+        <v>0.7719945678108373</v>
       </c>
       <c r="O4">
-        <v>1.100000023839263</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>0.826836754355374</v>
+        <v>0.7719945678096874</v>
       </c>
       <c r="Q4">
-        <v>41.92164926482276</v>
+        <v>-6.619958059522241</v>
       </c>
       <c r="R4">
-        <v>-89.9999999999964</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>123.7614475143174</v>
+        <v>173.3800419405132</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -5920,58 +5920,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>1.780157175146008</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>2.314120905097127</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1.728412445116581</v>
       </c>
       <c r="E5">
-        <v>20.55548448540783</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>26.72116654990333</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>19.95798780917515</v>
       </c>
       <c r="H5">
-        <v>7.895175922947299</v>
+        <v>7.895175922947224</v>
       </c>
       <c r="I5">
-        <v>7.335082718453101</v>
+        <v>7.335082718453457</v>
       </c>
       <c r="J5">
-        <v>1.477816378913028</v>
+        <v>1.477816378918004</v>
       </c>
       <c r="K5">
-        <v>5.558163488980913</v>
+        <v>5.558163489027946</v>
       </c>
       <c r="L5">
-        <v>1.477816378891169</v>
+        <v>1.477816378890884</v>
       </c>
       <c r="M5">
-        <v>5.558163488980769</v>
+        <v>5.558163488980837</v>
       </c>
       <c r="N5">
-        <v>0.6175627786591099</v>
+        <v>0.7719945678108373</v>
       </c>
       <c r="O5">
-        <v>1.100000023839263</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>0.8268367543553737</v>
+        <v>0.7719945678096877</v>
       </c>
       <c r="Q5">
-        <v>41.92164926482278</v>
+        <v>-6.619958059522241</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999639</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>123.7614475143174</v>
+        <v>173.3800419405131</v>
       </c>
     </row>
   </sheetData>
@@ -6051,58 +6051,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>1.170817013876365</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1.170998762980853</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1.171492593911478</v>
       </c>
       <c r="E2">
-        <v>13.51943036266627</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>13.52152902055428</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>13.5272312889689</v>
       </c>
       <c r="H2">
-        <v>0.4428835862221607</v>
+        <v>0.4428835862221404</v>
       </c>
       <c r="I2">
-        <v>4.402719738519057</v>
+        <v>4.40271973851942</v>
       </c>
       <c r="J2">
-        <v>0.437816356924225</v>
+        <v>0.4378163569293868</v>
       </c>
       <c r="K2">
-        <v>4.378163482487345</v>
+        <v>4.378163482534344</v>
       </c>
       <c r="L2">
-        <v>0.4378163569023265</v>
+        <v>0.4378163569022844</v>
       </c>
       <c r="M2">
-        <v>4.378163482487091</v>
+        <v>4.378163482487168</v>
       </c>
       <c r="N2">
-        <v>0.8440341447457987</v>
+        <v>0.9729578720439175</v>
       </c>
       <c r="O2">
-        <v>1.100000023840153</v>
+        <v>0.7175004542770153</v>
       </c>
       <c r="P2">
-        <v>0.9727947881380373</v>
+        <v>0.8439035640961189</v>
       </c>
       <c r="Q2">
-        <v>31.7119228523478</v>
+        <v>17.56327454668237</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999653</v>
+        <v>-104.8932091443124</v>
       </c>
       <c r="S2">
-        <v>137.5699449588465</v>
+        <v>151.7220699253674</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -6110,58 +6110,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>1.020468705618021</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1.10849935256055</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1.010036008422979</v>
       </c>
       <c r="E3">
-        <v>11.78335763776307</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>12.79984799194719</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>11.66289122708445</v>
       </c>
       <c r="H3">
-        <v>4.185910274912456</v>
+        <v>4.185910274912399</v>
       </c>
       <c r="I3">
-        <v>5.870495034005926</v>
+        <v>5.870495034006284</v>
       </c>
       <c r="J3">
-        <v>0.9578163680481669</v>
+        <v>0.9578163680532483</v>
       </c>
       <c r="K3">
-        <v>4.968163485594707</v>
+        <v>4.968163485641733</v>
       </c>
       <c r="L3">
-        <v>0.9578163680263008</v>
+        <v>0.9578163680261339</v>
       </c>
       <c r="M3">
-        <v>4.968163485594511</v>
+        <v>4.968163485594578</v>
       </c>
       <c r="N3">
-        <v>0.8440065675549148</v>
+        <v>0.9653165427949276</v>
       </c>
       <c r="O3">
-        <v>1.100000023840383</v>
+        <v>0.669786432244013</v>
       </c>
       <c r="P3">
-        <v>0.9689144874145577</v>
+        <v>0.8518280946068217</v>
       </c>
       <c r="Q3">
-        <v>31.98508613615191</v>
+        <v>16.29079354750229</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999645</v>
+        <v>-104.1338952714761</v>
       </c>
       <c r="S3">
-        <v>137.6328508700616</v>
+        <v>153.6019224867848</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -6169,58 +6169,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.9013413882071819</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1.040334427153928</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.9016673918744195</v>
       </c>
       <c r="E4">
-        <v>10.40779386226335</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>12.01274723129111</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>10.41155822836408</v>
       </c>
       <c r="H4">
-        <v>7.895175922947306</v>
+        <v>7.895175922947225</v>
       </c>
       <c r="I4">
-        <v>7.335082718453107</v>
+        <v>7.335082718453467</v>
       </c>
       <c r="J4">
-        <v>1.477816378913027</v>
+        <v>1.477816378918005</v>
       </c>
       <c r="K4">
-        <v>5.558163488980915</v>
+        <v>5.558163489027947</v>
       </c>
       <c r="L4">
-        <v>1.477816378891169</v>
+        <v>1.477816378890885</v>
       </c>
       <c r="M4">
-        <v>5.558163488980771</v>
+        <v>5.558163488980837</v>
       </c>
       <c r="N4">
-        <v>0.8434715680207194</v>
+        <v>0.9579198071587197</v>
       </c>
       <c r="O4">
-        <v>1.100000023840569</v>
+        <v>0.6279322069792089</v>
       </c>
       <c r="P4">
-        <v>0.9656494086163243</v>
+        <v>0.8564846443872474</v>
       </c>
       <c r="Q4">
-        <v>32.20512181945389</v>
+        <v>15.26462421738486</v>
       </c>
       <c r="R4">
-        <v>-89.9999999999964</v>
+        <v>-103.4693739255812</v>
       </c>
       <c r="S4">
-        <v>137.6537678120567</v>
+        <v>155.2583730680015</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -6228,58 +6228,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.9013413882071819</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1.040334427153928</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.9016673918744195</v>
       </c>
       <c r="E5">
-        <v>10.40779386226335</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>12.01274723129111</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>10.41155822836408</v>
       </c>
       <c r="H5">
-        <v>7.895175922947299</v>
+        <v>7.895175922947224</v>
       </c>
       <c r="I5">
-        <v>7.335082718453101</v>
+        <v>7.335082718453457</v>
       </c>
       <c r="J5">
-        <v>1.477816378913028</v>
+        <v>1.477816378918004</v>
       </c>
       <c r="K5">
-        <v>5.558163488980913</v>
+        <v>5.558163489027946</v>
       </c>
       <c r="L5">
-        <v>1.477816378891169</v>
+        <v>1.477816378890884</v>
       </c>
       <c r="M5">
-        <v>5.558163488980769</v>
+        <v>5.558163488980837</v>
       </c>
       <c r="N5">
-        <v>0.8434715680207194</v>
+        <v>0.9579198071587198</v>
       </c>
       <c r="O5">
-        <v>1.100000023840569</v>
+        <v>0.627932206979209</v>
       </c>
       <c r="P5">
-        <v>0.9656494086163243</v>
+        <v>0.8564846443872474</v>
       </c>
       <c r="Q5">
-        <v>32.20512181945389</v>
+        <v>15.26462421738487</v>
       </c>
       <c r="R5">
-        <v>-89.9999999999964</v>
+        <v>-103.4693739255812</v>
       </c>
       <c r="S5">
-        <v>137.6537678120567</v>
+        <v>155.2583730680015</v>
       </c>
     </row>
   </sheetData>
@@ -6359,58 +6359,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>1.170817013876365</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1.170998762980853</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1.171492593911478</v>
       </c>
       <c r="E2">
-        <v>13.51943036266627</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>13.52152902055428</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>13.5272312889689</v>
       </c>
       <c r="H2">
-        <v>0.4428835862221607</v>
+        <v>0.4428835862221404</v>
       </c>
       <c r="I2">
-        <v>4.402719738519057</v>
+        <v>4.40271973851942</v>
       </c>
       <c r="J2">
-        <v>0.437816356924225</v>
+        <v>0.4378163569293868</v>
       </c>
       <c r="K2">
-        <v>4.378163482487345</v>
+        <v>4.378163482534344</v>
       </c>
       <c r="L2">
-        <v>0.4378163569023265</v>
+        <v>0.4378163569022844</v>
       </c>
       <c r="M2">
-        <v>4.378163482487091</v>
+        <v>4.378163482487168</v>
       </c>
       <c r="N2">
-        <v>0.8440341447457987</v>
+        <v>0.9729578720439175</v>
       </c>
       <c r="O2">
-        <v>1.100000023840153</v>
+        <v>0.7175004542770153</v>
       </c>
       <c r="P2">
-        <v>0.9727947881380373</v>
+        <v>0.8439035640961189</v>
       </c>
       <c r="Q2">
-        <v>31.7119228523478</v>
+        <v>17.56327454668237</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999653</v>
+        <v>-104.8932091443124</v>
       </c>
       <c r="S2">
-        <v>137.5699449588465</v>
+        <v>151.7220699253674</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -6418,58 +6418,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>1.020468705618021</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1.10849935256055</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1.010036008422979</v>
       </c>
       <c r="E3">
-        <v>11.78335763776307</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>12.79984799194719</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>11.66289122708445</v>
       </c>
       <c r="H3">
-        <v>4.185910274912456</v>
+        <v>4.185910274912399</v>
       </c>
       <c r="I3">
-        <v>5.870495034005926</v>
+        <v>5.870495034006284</v>
       </c>
       <c r="J3">
-        <v>0.9578163680481669</v>
+        <v>0.9578163680532483</v>
       </c>
       <c r="K3">
-        <v>4.968163485594707</v>
+        <v>4.968163485641733</v>
       </c>
       <c r="L3">
-        <v>0.9578163680263008</v>
+        <v>0.9578163680261339</v>
       </c>
       <c r="M3">
-        <v>4.968163485594511</v>
+        <v>4.968163485594578</v>
       </c>
       <c r="N3">
-        <v>0.8440065675549148</v>
+        <v>0.9653165427949276</v>
       </c>
       <c r="O3">
-        <v>1.100000023840383</v>
+        <v>0.669786432244013</v>
       </c>
       <c r="P3">
-        <v>0.9689144874145577</v>
+        <v>0.8518280946068217</v>
       </c>
       <c r="Q3">
-        <v>31.98508613615191</v>
+        <v>16.29079354750229</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999645</v>
+        <v>-104.1338952714761</v>
       </c>
       <c r="S3">
-        <v>137.6328508700616</v>
+        <v>153.6019224867848</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -6477,58 +6477,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.9013413882071819</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1.040334427153928</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.9016673918744195</v>
       </c>
       <c r="E4">
-        <v>10.40779386226335</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>12.01274723129111</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>10.41155822836408</v>
       </c>
       <c r="H4">
-        <v>7.895175922947306</v>
+        <v>7.895175922947225</v>
       </c>
       <c r="I4">
-        <v>7.335082718453107</v>
+        <v>7.335082718453467</v>
       </c>
       <c r="J4">
-        <v>1.477816378913027</v>
+        <v>1.477816378918005</v>
       </c>
       <c r="K4">
-        <v>5.558163488980915</v>
+        <v>5.558163489027947</v>
       </c>
       <c r="L4">
-        <v>1.477816378891169</v>
+        <v>1.477816378890885</v>
       </c>
       <c r="M4">
-        <v>5.558163488980771</v>
+        <v>5.558163488980837</v>
       </c>
       <c r="N4">
-        <v>0.8434715680207194</v>
+        <v>0.9579198071587197</v>
       </c>
       <c r="O4">
-        <v>1.100000023840569</v>
+        <v>0.6279322069792089</v>
       </c>
       <c r="P4">
-        <v>0.9656494086163243</v>
+        <v>0.8564846443872474</v>
       </c>
       <c r="Q4">
-        <v>32.20512181945389</v>
+        <v>15.26462421738486</v>
       </c>
       <c r="R4">
-        <v>-89.9999999999964</v>
+        <v>-103.4693739255812</v>
       </c>
       <c r="S4">
-        <v>137.6537678120567</v>
+        <v>155.2583730680015</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -6536,58 +6536,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.9013413882071819</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1.040334427153928</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.9016673918744195</v>
       </c>
       <c r="E5">
-        <v>10.40779386226335</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>12.01274723129111</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>10.41155822836408</v>
       </c>
       <c r="H5">
-        <v>7.895175922947299</v>
+        <v>7.895175922947224</v>
       </c>
       <c r="I5">
-        <v>7.335082718453101</v>
+        <v>7.335082718453457</v>
       </c>
       <c r="J5">
-        <v>1.477816378913028</v>
+        <v>1.477816378918004</v>
       </c>
       <c r="K5">
-        <v>5.558163488980913</v>
+        <v>5.558163489027946</v>
       </c>
       <c r="L5">
-        <v>1.477816378891169</v>
+        <v>1.477816378890884</v>
       </c>
       <c r="M5">
-        <v>5.558163488980769</v>
+        <v>5.558163488980837</v>
       </c>
       <c r="N5">
-        <v>0.8434715680207194</v>
+        <v>0.9579198071587198</v>
       </c>
       <c r="O5">
-        <v>1.100000023840569</v>
+        <v>0.627932206979209</v>
       </c>
       <c r="P5">
-        <v>0.9656494086163243</v>
+        <v>0.8564846443872474</v>
       </c>
       <c r="Q5">
-        <v>32.20512181945389</v>
+        <v>15.26462421738487</v>
       </c>
       <c r="R5">
-        <v>-89.9999999999964</v>
+        <v>-103.4693739255812</v>
       </c>
       <c r="S5">
-        <v>137.6537678120567</v>
+        <v>155.2583730680015</v>
       </c>
     </row>
   </sheetData>
@@ -6667,58 +6667,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>2.304451709204056</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2.307394468727928</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2.306476761395013</v>
       </c>
       <c r="E2">
-        <v>26.6095162928691</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>26.64349635293446</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>26.63289958142054</v>
       </c>
       <c r="H2">
-        <v>0.5041743431842567</v>
+        <v>0.5041743431842544</v>
       </c>
       <c r="I2">
-        <v>5.006897135806157</v>
+        <v>5.006897135806584</v>
       </c>
       <c r="J2">
-        <v>0.4975185876920994</v>
+        <v>0.4975185876946874</v>
       </c>
       <c r="K2">
-        <v>4.975185775488431</v>
+        <v>4.975185775457811</v>
       </c>
       <c r="L2">
-        <v>0.497518587712459</v>
+        <v>0.4975185877124232</v>
       </c>
       <c r="M2">
-        <v>4.97518577548815</v>
+        <v>4.975185775488254</v>
       </c>
       <c r="N2">
-        <v>0.5778549958900403</v>
+        <v>0.5785850458643943</v>
       </c>
       <c r="O2">
-        <v>0.9999999999962847</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0.5780849144276639</v>
+        <v>0.5785850458648649</v>
       </c>
       <c r="Q2">
-        <v>59.88716006626888</v>
+        <v>-0.01310313119137088</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999636</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>120.0996242896476</v>
+        <v>179.9868968685288</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -6726,58 +6726,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>1.684845595525955</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2.144785402460348</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1.543474101037902</v>
       </c>
       <c r="E3">
-        <v>19.45492116239731</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>24.76584858928923</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>17.82250375442897</v>
       </c>
       <c r="H3">
-        <v>7.698542227644828</v>
+        <v>7.698542227644789</v>
       </c>
       <c r="I3">
-        <v>6.432196710718991</v>
+        <v>6.432196710719398</v>
       </c>
       <c r="J3">
-        <v>1.495918608640806</v>
+        <v>1.495918608642645</v>
       </c>
       <c r="K3">
-        <v>5.565185778099434</v>
+        <v>5.565185778068525</v>
       </c>
       <c r="L3">
-        <v>1.495918608660816</v>
+        <v>1.495918608660561</v>
       </c>
       <c r="M3">
-        <v>5.565185778099255</v>
+        <v>5.565185778099361</v>
       </c>
       <c r="N3">
-        <v>0.5407731743511122</v>
+        <v>0.6950234972340792</v>
       </c>
       <c r="O3">
-        <v>0.9999999999980868</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>0.7514492206972073</v>
+        <v>0.6950234972340121</v>
       </c>
       <c r="Q3">
-        <v>42.2903649473445</v>
+        <v>-7.611827049086783</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999652</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>122.1643601284607</v>
+        <v>172.3881729507654</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -6785,58 +6785,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>1.224899235816899</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1.791382665021896</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1.312244351459671</v>
       </c>
       <c r="E4">
-        <v>14.14391807058107</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>20.68510527744042</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>15.15249259115614</v>
       </c>
       <c r="H4">
-        <v>14.82177840037519</v>
+        <v>14.8217784003751</v>
       </c>
       <c r="I4">
-        <v>7.872438169825329</v>
+        <v>7.872438169825732</v>
       </c>
       <c r="J4">
-        <v>2.494318629320983</v>
+        <v>2.494318629322498</v>
       </c>
       <c r="K4">
-        <v>6.155185781289128</v>
+        <v>6.155185781258161</v>
       </c>
       <c r="L4">
-        <v>2.494318629340928</v>
+        <v>2.494318629340454</v>
       </c>
       <c r="M4">
-        <v>6.155185781289043</v>
+        <v>6.155185781289154</v>
       </c>
       <c r="N4">
-        <v>0.5992308608385498</v>
+        <v>0.7474500608991325</v>
       </c>
       <c r="O4">
-        <v>0.9999999999990241</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>0.8180273553921663</v>
+        <v>0.7474500608986431</v>
       </c>
       <c r="Q4">
-        <v>35.14600558028982</v>
+        <v>-6.297561754805892</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999639</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>126.7970300907754</v>
+        <v>173.702438245086</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -6844,58 +6844,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>1.224899235816899</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1.791382665021898</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1.31224435145967</v>
       </c>
       <c r="E5">
-        <v>14.14391807058107</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>20.68510527744045</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>15.15249259115612</v>
       </c>
       <c r="H5">
-        <v>14.82177840037519</v>
+        <v>14.82177840037509</v>
       </c>
       <c r="I5">
-        <v>7.872438169825323</v>
+        <v>7.872438169825724</v>
       </c>
       <c r="J5">
-        <v>2.494318629320986</v>
+        <v>2.494318629322495</v>
       </c>
       <c r="K5">
-        <v>6.155185781289128</v>
+        <v>6.155185781258152</v>
       </c>
       <c r="L5">
-        <v>2.494318629340926</v>
+        <v>2.494318629340448</v>
       </c>
       <c r="M5">
-        <v>6.155185781289043</v>
+        <v>6.15518578128915</v>
       </c>
       <c r="N5">
-        <v>0.5992308608385494</v>
+        <v>0.7474500608991327</v>
       </c>
       <c r="O5">
-        <v>0.9999999999990241</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>0.8180273553921662</v>
+        <v>0.7474500608986436</v>
       </c>
       <c r="Q5">
-        <v>35.14600558028984</v>
+        <v>-6.297561754805924</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999639</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>126.7970300907753</v>
+        <v>173.702438245086</v>
       </c>
     </row>
   </sheetData>
@@ -7103,58 +7103,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>2.304451709204056</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2.307394468727928</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2.306476761395013</v>
       </c>
       <c r="E2">
-        <v>26.6095162928691</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>26.64349635293446</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>26.63289958142054</v>
       </c>
       <c r="H2">
-        <v>0.5041743431842567</v>
+        <v>0.5041743431842544</v>
       </c>
       <c r="I2">
-        <v>5.006897135806157</v>
+        <v>5.006897135806584</v>
       </c>
       <c r="J2">
-        <v>0.4975185876920994</v>
+        <v>0.4975185876946874</v>
       </c>
       <c r="K2">
-        <v>4.975185775488431</v>
+        <v>4.975185775457811</v>
       </c>
       <c r="L2">
-        <v>0.497518587712459</v>
+        <v>0.4975185877124232</v>
       </c>
       <c r="M2">
-        <v>4.97518577548815</v>
+        <v>4.975185775488254</v>
       </c>
       <c r="N2">
-        <v>0.5778549958900403</v>
+        <v>0.5785850458643943</v>
       </c>
       <c r="O2">
-        <v>0.9999999999962847</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0.5780849144276639</v>
+        <v>0.5785850458648649</v>
       </c>
       <c r="Q2">
-        <v>59.88716006626888</v>
+        <v>-0.01310313119137088</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999636</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>120.0996242896476</v>
+        <v>179.9868968685288</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -7162,58 +7162,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>1.684845595525955</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2.144785402460348</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1.543474101037902</v>
       </c>
       <c r="E3">
-        <v>19.45492116239731</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>24.76584858928923</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>17.82250375442897</v>
       </c>
       <c r="H3">
-        <v>7.698542227644828</v>
+        <v>7.698542227644789</v>
       </c>
       <c r="I3">
-        <v>6.432196710718991</v>
+        <v>6.432196710719398</v>
       </c>
       <c r="J3">
-        <v>1.495918608640806</v>
+        <v>1.495918608642645</v>
       </c>
       <c r="K3">
-        <v>5.565185778099434</v>
+        <v>5.565185778068525</v>
       </c>
       <c r="L3">
-        <v>1.495918608660816</v>
+        <v>1.495918608660561</v>
       </c>
       <c r="M3">
-        <v>5.565185778099255</v>
+        <v>5.565185778099361</v>
       </c>
       <c r="N3">
-        <v>0.5407731743511122</v>
+        <v>0.6950234972340792</v>
       </c>
       <c r="O3">
-        <v>0.9999999999980868</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>0.7514492206972073</v>
+        <v>0.6950234972340121</v>
       </c>
       <c r="Q3">
-        <v>42.2903649473445</v>
+        <v>-7.611827049086783</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999652</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>122.1643601284607</v>
+        <v>172.3881729507654</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -7221,58 +7221,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>1.224899235816899</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1.791382665021896</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1.312244351459671</v>
       </c>
       <c r="E4">
-        <v>14.14391807058107</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>20.68510527744042</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>15.15249259115614</v>
       </c>
       <c r="H4">
-        <v>14.82177840037519</v>
+        <v>14.8217784003751</v>
       </c>
       <c r="I4">
-        <v>7.872438169825329</v>
+        <v>7.872438169825732</v>
       </c>
       <c r="J4">
-        <v>2.494318629320983</v>
+        <v>2.494318629322498</v>
       </c>
       <c r="K4">
-        <v>6.155185781289128</v>
+        <v>6.155185781258161</v>
       </c>
       <c r="L4">
-        <v>2.494318629340928</v>
+        <v>2.494318629340454</v>
       </c>
       <c r="M4">
-        <v>6.155185781289043</v>
+        <v>6.155185781289154</v>
       </c>
       <c r="N4">
-        <v>0.5992308608385498</v>
+        <v>0.7474500608991325</v>
       </c>
       <c r="O4">
-        <v>0.9999999999990241</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>0.8180273553921663</v>
+        <v>0.7474500608986431</v>
       </c>
       <c r="Q4">
-        <v>35.14600558028982</v>
+        <v>-6.297561754805892</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999639</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>126.7970300907754</v>
+        <v>173.702438245086</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -7280,58 +7280,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>1.224899235816899</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1.791382665021898</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1.31224435145967</v>
       </c>
       <c r="E5">
-        <v>14.14391807058107</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>20.68510527744045</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>15.15249259115612</v>
       </c>
       <c r="H5">
-        <v>14.82177840037519</v>
+        <v>14.82177840037509</v>
       </c>
       <c r="I5">
-        <v>7.872438169825323</v>
+        <v>7.872438169825724</v>
       </c>
       <c r="J5">
-        <v>2.494318629320986</v>
+        <v>2.494318629322495</v>
       </c>
       <c r="K5">
-        <v>6.155185781289128</v>
+        <v>6.155185781258152</v>
       </c>
       <c r="L5">
-        <v>2.494318629340926</v>
+        <v>2.494318629340448</v>
       </c>
       <c r="M5">
-        <v>6.155185781289043</v>
+        <v>6.15518578128915</v>
       </c>
       <c r="N5">
-        <v>0.5992308608385494</v>
+        <v>0.7474500608991327</v>
       </c>
       <c r="O5">
-        <v>0.9999999999990241</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>0.8180273553921662</v>
+        <v>0.7474500608986436</v>
       </c>
       <c r="Q5">
-        <v>35.14600558028984</v>
+        <v>-6.297561754805924</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999639</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>126.7970300907753</v>
+        <v>173.702438245086</v>
       </c>
     </row>
   </sheetData>
@@ -7411,58 +7411,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>1.012885714576425</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1.013102923845676</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1.013588406235421</v>
       </c>
       <c r="E2">
-        <v>11.69579679938051</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>11.69830491598196</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>11.70391078375008</v>
       </c>
       <c r="H2">
-        <v>0.5041743431842567</v>
+        <v>0.5041743431842544</v>
       </c>
       <c r="I2">
-        <v>5.006897135806157</v>
+        <v>5.006897135806584</v>
       </c>
       <c r="J2">
-        <v>0.4975185876920994</v>
+        <v>0.4975185876946874</v>
       </c>
       <c r="K2">
-        <v>4.975185775488431</v>
+        <v>4.975185775457811</v>
       </c>
       <c r="L2">
-        <v>0.497518587712459</v>
+        <v>0.4975185877124232</v>
       </c>
       <c r="M2">
-        <v>4.97518577548815</v>
+        <v>4.975185775488254</v>
       </c>
       <c r="N2">
-        <v>0.7492067188226383</v>
+        <v>0.8721332518534242</v>
       </c>
       <c r="O2">
-        <v>0.9999999999987974</v>
+        <v>0.6208257825095037</v>
       </c>
       <c r="P2">
-        <v>0.8719401990676209</v>
+        <v>0.7490594668689452</v>
       </c>
       <c r="Q2">
-        <v>32.31584613269226</v>
+        <v>16.55576890986408</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999655</v>
+        <v>-106.1399873258002</v>
       </c>
       <c r="S2">
-        <v>136.5651455806771</v>
+        <v>152.3303371030605</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -7470,58 +7470,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.8351922431613388</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.9576169384185383</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.8150213495726398</v>
       </c>
       <c r="E3">
-        <v>9.643969328285728</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>11.05760794352977</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>9.411055911421114</v>
       </c>
       <c r="H3">
-        <v>7.698542227644828</v>
+        <v>7.698542227644789</v>
       </c>
       <c r="I3">
-        <v>6.432196710718991</v>
+        <v>6.432196710719398</v>
       </c>
       <c r="J3">
-        <v>1.495918608640806</v>
+        <v>1.495918608642645</v>
       </c>
       <c r="K3">
-        <v>5.565185778099434</v>
+        <v>5.565185778068525</v>
       </c>
       <c r="L3">
-        <v>1.495918608660816</v>
+        <v>1.495918608660561</v>
       </c>
       <c r="M3">
-        <v>5.565185778099255</v>
+        <v>5.565185778099361</v>
       </c>
       <c r="N3">
-        <v>0.7615594742962095</v>
+        <v>0.8671834304540896</v>
       </c>
       <c r="O3">
-        <v>0.9999999999991965</v>
+        <v>0.5701359740030982</v>
       </c>
       <c r="P3">
-        <v>0.877371251159636</v>
+        <v>0.7780446838807024</v>
       </c>
       <c r="Q3">
-        <v>32.13594383429049</v>
+        <v>15.07716951670869</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999645</v>
+        <v>-103.4150584572222</v>
       </c>
       <c r="S3">
-        <v>137.3083573823813</v>
+        <v>154.9843720112472</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -7529,58 +7529,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.6999120446284219</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.8779780941084492</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.7099194197390576</v>
       </c>
       <c r="E4">
-        <v>8.081888147505616</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>10.13801777952216</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>8.197443361785757</v>
       </c>
       <c r="H4">
-        <v>14.82177840037519</v>
+        <v>14.8217784003751</v>
       </c>
       <c r="I4">
-        <v>7.872438169825329</v>
+        <v>7.872438169825732</v>
       </c>
       <c r="J4">
-        <v>2.494318629320983</v>
+        <v>2.494318629322498</v>
       </c>
       <c r="K4">
-        <v>6.155185781289128</v>
+        <v>6.155185781258161</v>
       </c>
       <c r="L4">
-        <v>2.494318629340928</v>
+        <v>2.494318629340454</v>
       </c>
       <c r="M4">
-        <v>6.155185781289043</v>
+        <v>6.155185781289154</v>
       </c>
       <c r="N4">
-        <v>0.7700746676618133</v>
+        <v>0.8595183170292721</v>
       </c>
       <c r="O4">
-        <v>0.999999999999447</v>
+        <v>0.526165712950652</v>
       </c>
       <c r="P4">
-        <v>0.8785874061674938</v>
+        <v>0.793440478635774</v>
       </c>
       <c r="Q4">
-        <v>32.21715262800947</v>
+        <v>14.16121021104031</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999638</v>
+        <v>-101.1058570224848</v>
       </c>
       <c r="S4">
-        <v>137.8628958470784</v>
+        <v>157.3127817016637</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -7588,58 +7588,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.699912044628422</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.8779780941084497</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.7099194197390573</v>
       </c>
       <c r="E5">
-        <v>8.081888147505618</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>10.13801777952216</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>8.197443361785753</v>
       </c>
       <c r="H5">
-        <v>14.82177840037519</v>
+        <v>14.82177840037509</v>
       </c>
       <c r="I5">
-        <v>7.872438169825323</v>
+        <v>7.872438169825724</v>
       </c>
       <c r="J5">
-        <v>2.494318629320986</v>
+        <v>2.494318629322495</v>
       </c>
       <c r="K5">
-        <v>6.155185781289128</v>
+        <v>6.155185781258152</v>
       </c>
       <c r="L5">
-        <v>2.494318629340926</v>
+        <v>2.494318629340448</v>
       </c>
       <c r="M5">
-        <v>6.155185781289043</v>
+        <v>6.15518578128915</v>
       </c>
       <c r="N5">
-        <v>0.7700746676618129</v>
+        <v>0.8595183170292721</v>
       </c>
       <c r="O5">
-        <v>0.9999999999994468</v>
+        <v>0.526165712950652</v>
       </c>
       <c r="P5">
-        <v>0.8785874061674938</v>
+        <v>0.793440478635774</v>
       </c>
       <c r="Q5">
-        <v>32.21715262800947</v>
+        <v>14.1612102110403</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999636</v>
+        <v>-101.1058570224848</v>
       </c>
       <c r="S5">
-        <v>137.8628958470784</v>
+        <v>157.3127817016637</v>
       </c>
     </row>
   </sheetData>
@@ -7719,58 +7719,58 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>1.012885714576425</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1.013102923845676</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1.013588406235421</v>
       </c>
       <c r="E2">
-        <v>11.69579679938051</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>11.69830491598196</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>11.70391078375008</v>
       </c>
       <c r="H2">
-        <v>0.5041743431842567</v>
+        <v>0.5041743431842544</v>
       </c>
       <c r="I2">
-        <v>5.006897135806157</v>
+        <v>5.006897135806584</v>
       </c>
       <c r="J2">
-        <v>0.4975185876920994</v>
+        <v>0.4975185876946874</v>
       </c>
       <c r="K2">
-        <v>4.975185775488431</v>
+        <v>4.975185775457811</v>
       </c>
       <c r="L2">
-        <v>0.497518587712459</v>
+        <v>0.4975185877124232</v>
       </c>
       <c r="M2">
-        <v>4.97518577548815</v>
+        <v>4.975185775488254</v>
       </c>
       <c r="N2">
-        <v>0.7492067188226383</v>
+        <v>0.8721332518534242</v>
       </c>
       <c r="O2">
-        <v>0.9999999999987974</v>
+        <v>0.6208257825095037</v>
       </c>
       <c r="P2">
-        <v>0.8719401990676209</v>
+        <v>0.7490594668689452</v>
       </c>
       <c r="Q2">
-        <v>32.31584613269226</v>
+        <v>16.55576890986408</v>
       </c>
       <c r="R2">
-        <v>-89.99999999999655</v>
+        <v>-106.1399873258002</v>
       </c>
       <c r="S2">
-        <v>136.5651455806771</v>
+        <v>152.3303371030605</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -7778,58 +7778,58 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.8351922431613388</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.9576169384185383</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.8150213495726398</v>
       </c>
       <c r="E3">
-        <v>9.643969328285728</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>11.05760794352977</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>9.411055911421114</v>
       </c>
       <c r="H3">
-        <v>7.698542227644828</v>
+        <v>7.698542227644789</v>
       </c>
       <c r="I3">
-        <v>6.432196710718991</v>
+        <v>6.432196710719398</v>
       </c>
       <c r="J3">
-        <v>1.495918608640806</v>
+        <v>1.495918608642645</v>
       </c>
       <c r="K3">
-        <v>5.565185778099434</v>
+        <v>5.565185778068525</v>
       </c>
       <c r="L3">
-        <v>1.495918608660816</v>
+        <v>1.495918608660561</v>
       </c>
       <c r="M3">
-        <v>5.565185778099255</v>
+        <v>5.565185778099361</v>
       </c>
       <c r="N3">
-        <v>0.7615594742962095</v>
+        <v>0.8671834304540896</v>
       </c>
       <c r="O3">
-        <v>0.9999999999991965</v>
+        <v>0.5701359740030982</v>
       </c>
       <c r="P3">
-        <v>0.877371251159636</v>
+        <v>0.7780446838807024</v>
       </c>
       <c r="Q3">
-        <v>32.13594383429049</v>
+        <v>15.07716951670869</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999645</v>
+        <v>-103.4150584572222</v>
       </c>
       <c r="S3">
-        <v>137.3083573823813</v>
+        <v>154.9843720112472</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -7837,58 +7837,58 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.6999120446284219</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.8779780941084492</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.7099194197390576</v>
       </c>
       <c r="E4">
-        <v>8.081888147505616</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>10.13801777952216</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>8.197443361785757</v>
       </c>
       <c r="H4">
-        <v>14.82177840037519</v>
+        <v>14.8217784003751</v>
       </c>
       <c r="I4">
-        <v>7.872438169825329</v>
+        <v>7.872438169825732</v>
       </c>
       <c r="J4">
-        <v>2.494318629320983</v>
+        <v>2.494318629322498</v>
       </c>
       <c r="K4">
-        <v>6.155185781289128</v>
+        <v>6.155185781258161</v>
       </c>
       <c r="L4">
-        <v>2.494318629340928</v>
+        <v>2.494318629340454</v>
       </c>
       <c r="M4">
-        <v>6.155185781289043</v>
+        <v>6.155185781289154</v>
       </c>
       <c r="N4">
-        <v>0.7700746676618133</v>
+        <v>0.8595183170292721</v>
       </c>
       <c r="O4">
-        <v>0.999999999999447</v>
+        <v>0.526165712950652</v>
       </c>
       <c r="P4">
-        <v>0.8785874061674938</v>
+        <v>0.793440478635774</v>
       </c>
       <c r="Q4">
-        <v>32.21715262800947</v>
+        <v>14.16121021104031</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999638</v>
+        <v>-101.1058570224848</v>
       </c>
       <c r="S4">
-        <v>137.8628958470784</v>
+        <v>157.3127817016637</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -7896,58 +7896,58 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.699912044628422</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.8779780941084497</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.7099194197390573</v>
       </c>
       <c r="E5">
-        <v>8.081888147505618</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>10.13801777952216</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>8.197443361785753</v>
       </c>
       <c r="H5">
-        <v>14.82177840037519</v>
+        <v>14.82177840037509</v>
       </c>
       <c r="I5">
-        <v>7.872438169825323</v>
+        <v>7.872438169825724</v>
       </c>
       <c r="J5">
-        <v>2.494318629320986</v>
+        <v>2.494318629322495</v>
       </c>
       <c r="K5">
-        <v>6.155185781289128</v>
+        <v>6.155185781258152</v>
       </c>
       <c r="L5">
-        <v>2.494318629340926</v>
+        <v>2.494318629340448</v>
       </c>
       <c r="M5">
-        <v>6.155185781289043</v>
+        <v>6.15518578128915</v>
       </c>
       <c r="N5">
-        <v>0.7700746676618129</v>
+        <v>0.8595183170292721</v>
       </c>
       <c r="O5">
-        <v>0.9999999999994468</v>
+        <v>0.526165712950652</v>
       </c>
       <c r="P5">
-        <v>0.8785874061674938</v>
+        <v>0.793440478635774</v>
       </c>
       <c r="Q5">
-        <v>32.21715262800947</v>
+        <v>14.1612102110403</v>
       </c>
       <c r="R5">
-        <v>-89.99999999999636</v>
+        <v>-101.1058570224848</v>
       </c>
       <c r="S5">
-        <v>137.8628958470784</v>
+        <v>157.3127817016637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>